<commit_message>
Add all experiment charts
</commit_message>
<xml_diff>
--- a/charts/measurements format.xlsx
+++ b/charts/measurements format.xlsx
@@ -63,6 +63,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -229,7 +230,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -297,6 +298,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="0" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -579,6 +581,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="0" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -831,11 +834,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="54808789"/>
-        <c:axId val="36716738"/>
+        <c:axId val="79602392"/>
+        <c:axId val="95954155"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54808789"/>
+        <c:axId val="79602392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13"/>
@@ -879,7 +882,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -901,13 +904,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36716738"/>
+        <c:crossAx val="95954155"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36716738"/>
+        <c:axId val="95954155"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -950,7 +953,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -972,7 +975,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54808789"/>
+        <c:crossAx val="79602392"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1031,9 +1034,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>559080</xdr:colOff>
+      <xdr:colOff>558720</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1041,8 +1044,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2877840" y="1861200"/>
-        <a:ext cx="7094160" cy="3809520"/>
+        <a:off x="2878560" y="1861200"/>
+        <a:ext cx="7093800" cy="3809160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1060,16 +1063,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P91"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F102" activeCellId="0" sqref="F99:F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="11.52"/>
@@ -4179,6 +4182,26 @@
         <v>61.893049382716</v>
       </c>
     </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G99" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G100" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G101" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G102" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>